<commit_message>
changed blank slots back to blank
</commit_message>
<xml_diff>
--- a/SanitizedVoteData_05022021.xlsx
+++ b/SanitizedVoteData_05022021.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="35">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">V2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C8</t>
   </si>
   <si>
     <t xml:space="preserve">V3</t>
@@ -229,7 +226,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,6 +241,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -333,11 +334,11 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5 F10 F15:F16 G7 G17 H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.75" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="333" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -369,7 +370,7 @@
       <c r="A2" s="3" t="n">
         <v>44321.8152430556</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -395,7 +396,7 @@
       <c r="A3" s="3" t="n">
         <v>44321.8154398148</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -407,22 +408,18 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>44321.8154398148</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>17</v>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -434,21 +431,21 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>44321.815474537</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>20</v>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -460,7 +457,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -473,8 +470,8 @@
       <c r="A6" s="3" t="n">
         <v>44321.8156018519</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>21</v>
+      <c r="B6" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -492,15 +489,15 @@
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>44321.8156597222</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>22</v>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
@@ -515,18 +512,18 @@
         <v>13</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>44321.8157638889</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>23</v>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
@@ -538,7 +535,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>13</v>
@@ -551,8 +548,8 @@
       <c r="A9" s="3" t="n">
         <v>44321.815775463</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>24</v>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -564,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
@@ -577,8 +574,8 @@
       <c r="A10" s="3" t="n">
         <v>44321.8159490741</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>25</v>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
@@ -590,21 +587,21 @@
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
         <v>44321.8161805556</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>26</v>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
@@ -615,22 +612,16 @@
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>44321.8161921296</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>27</v>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -639,7 +630,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
@@ -655,8 +646,8 @@
       <c r="A13" s="3" t="n">
         <v>44321.8161921296</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>28</v>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
@@ -671,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>14</v>
@@ -681,8 +672,8 @@
       <c r="A14" s="3" t="n">
         <v>44321.8162847222</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>29</v>
+      <c r="B14" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -700,15 +691,15 @@
         <v>14</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <v>44321.8164467593</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>30</v>
+      <c r="B15" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
@@ -720,33 +711,33 @@
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <v>44321.8165277778</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>31</v>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>13</v>
@@ -759,8 +750,8 @@
       <c r="A17" s="3" t="n">
         <v>44321.8166666667</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>32</v>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -775,7 +766,7 @@
         <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>12</v>
@@ -785,8 +776,8 @@
       <c r="A18" s="3" t="n">
         <v>44321.8169791667</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>33</v>
+      <c r="B18" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
@@ -800,19 +791,15 @@
       <c r="F18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
         <v>44321.8191782407</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>34</v>
+      <c r="B19" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
@@ -821,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
@@ -837,8 +824,8 @@
       <c r="A20" s="3" t="n">
         <v>44321.8182638889</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>35</v>
+      <c r="B20" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
@@ -852,12 +839,8 @@
       <c r="F20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
@@ -941,7 +924,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>

</xml_diff>